<commit_message>
updated fio Excel graphs with error bars
</commit_message>
<xml_diff>
--- a/fio/results/fio results.xlsx
+++ b/fio/results/fio results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23515"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="20860" yWindow="4860" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
+    <workbookView xWindow="3580" yWindow="0" windowWidth="25040" windowHeight="15500" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -151,6 +151,41 @@
             </c:strRef>
           </c:tx>
           <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Sheet1!$C$6:$C$7</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="2"/>
+                  <c:pt idx="0">
+                    <c:v>0.37</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>14.579</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Sheet1!$C$6:$C$7</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="2"/>
+                  <c:pt idx="0">
+                    <c:v>0.37</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>14.579</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+          </c:errBars>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$A$6:$A$7</c:f>
@@ -196,6 +231,41 @@
             </c:strRef>
           </c:tx>
           <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Sheet1!$E$6:$E$7</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="2"/>
+                  <c:pt idx="0">
+                    <c:v>0.894</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>12.505</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Sheet1!$E$6:$E$7</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="2"/>
+                  <c:pt idx="0">
+                    <c:v>0.894</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>12.505</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+          </c:errBars>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$A$6:$A$7</c:f>
@@ -241,6 +311,41 @@
             </c:strRef>
           </c:tx>
           <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Sheet1!$G$6:$G$7</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="2"/>
+                  <c:pt idx="0">
+                    <c:v>4.019</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>60.383</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Sheet1!$G$6:$G$7</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="2"/>
+                  <c:pt idx="0">
+                    <c:v>4.019</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>60.383</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+          </c:errBars>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$A$6:$A$7</c:f>
@@ -280,11 +385,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2141957624"/>
-        <c:axId val="-2141954488"/>
+        <c:axId val="2092019976"/>
+        <c:axId val="2092022952"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2141957624"/>
+        <c:axId val="2092019976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -293,7 +398,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2141954488"/>
+        <c:crossAx val="2092022952"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -301,7 +406,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2141954488"/>
+        <c:axId val="2092022952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -313,7 +418,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2141957624"/>
+        <c:crossAx val="2092019976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:minorUnit val="100.0"/>
@@ -528,11 +633,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2139415416"/>
-        <c:axId val="-2139925320"/>
+        <c:axId val="2102915144"/>
+        <c:axId val="2102903960"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2139415416"/>
+        <c:axId val="2102915144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -541,7 +646,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2139925320"/>
+        <c:crossAx val="2102903960"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -549,7 +654,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2139925320"/>
+        <c:axId val="2102903960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -560,7 +665,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2139415416"/>
+        <c:crossAx val="2102915144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -965,11 +1070,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2136829320"/>
-        <c:axId val="-2140264264"/>
+        <c:axId val="2092793064"/>
+        <c:axId val="2092356056"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2136829320"/>
+        <c:axId val="2092793064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -979,12 +1084,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2140264264"/>
+        <c:crossAx val="2092356056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2140264264"/>
+        <c:axId val="2092356056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -995,7 +1100,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2136829320"/>
+        <c:crossAx val="2092793064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1031,15 +1136,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>325120</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>144780</xdr:rowOff>
+      <xdr:colOff>447040</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>43180</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>701040</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>158750</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1061,15 +1166,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
+      <xdr:colOff>71120</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>539750</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
+      <xdr:colOff>458470</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1450,7 +1555,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:L8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>

</xml_diff>